<commit_message>
adding a simple excel sheet for demo
</commit_message>
<xml_diff>
--- a/static/input_files/acfrs/example_template.xlsx
+++ b/static/input_files/acfrs/example_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5531B00-12A0-3144-9C9C-F84F065B1229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD601F11-7289-A647-BE96-0163B49465BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-9360" windowWidth="28160" windowHeight="21600" tabRatio="834" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13266,7 +13266,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
first stab at parsing statement of activities
</commit_message>
<xml_diff>
--- a/static/input_files/acfrs/example_template.xlsx
+++ b/static/input_files/acfrs/example_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9489C06-BF10-7144-B4DF-281ED8216F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D807F27-77E8-D543-A613-6F1476C70B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="500" windowWidth="24180" windowHeight="17500" tabRatio="834" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16900,8 +16900,8 @@
   </sheetPr>
   <dimension ref="A1:J99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -17045,18 +17045,12 @@
         <f>IF(OR(G$6="", B9=""),"",SUM(E9:F9) - C9)</f>
         <v/>
       </c>
-      <c r="H9" s="65" t="str">
-        <f>IF(OR(H$6="", $B9=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="H9" s="65"/>
       <c r="I9" s="17" t="str">
         <f>IF(OR($E$6="", B9=""),"",SUM(G9:H9))</f>
         <v/>
       </c>
-      <c r="J9" s="65" t="str">
-        <f>IF(OR(J$6="", $B9=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="J9" s="65"/>
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="8" t="str">
@@ -17072,18 +17066,12 @@
         <f>IF(OR(G$6="", B10=""),"",SUM(E10:F10) - C10)</f>
         <v/>
       </c>
-      <c r="H10" s="65" t="str">
-        <f>IF(OR(H$6="", $B10=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="H10" s="65"/>
       <c r="I10" s="17" t="str">
         <f>IF(OR($E$6="", B10=""),"",SUM(G10:H10))</f>
         <v/>
       </c>
-      <c r="J10" s="65" t="str">
-        <f>IF(OR(J$6="", $B10=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="J10" s="65"/>
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="8" t="str">
@@ -17099,18 +17087,12 @@
         <f t="shared" ref="G11:G22" si="0">IF(OR(G$6="", B11=""),"",SUM(E11:F11) - C11)</f>
         <v/>
       </c>
-      <c r="H11" s="65" t="str">
-        <f t="shared" ref="H11:H22" si="1">IF(OR(H$6="", $B11=""),"",0)</f>
+      <c r="H11" s="65"/>
+      <c r="I11" s="17" t="str">
+        <f t="shared" ref="I10:I22" si="1">IF(OR($E$6="", B11=""),"",SUM(G11:H11))</f>
         <v/>
       </c>
-      <c r="I11" s="17" t="str">
-        <f t="shared" ref="I10:I22" si="2">IF(OR($E$6="", B11=""),"",SUM(G11:H11))</f>
-        <v/>
-      </c>
-      <c r="J11" s="65" t="str">
-        <f t="shared" ref="J11:J22" si="3">IF(OR(J$6="", $B11=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="J11" s="65"/>
     </row>
     <row r="12" spans="1:10" ht="15">
       <c r="A12" s="8" t="str">
@@ -17126,18 +17108,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H12" s="65" t="str">
+      <c r="H12" s="65"/>
+      <c r="I12" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I12" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J12" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J12" s="65"/>
     </row>
     <row r="13" spans="1:10" ht="15">
       <c r="A13" s="8" t="str">
@@ -17153,18 +17129,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H13" s="65" t="str">
+      <c r="H13" s="65"/>
+      <c r="I13" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I13" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J13" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J13" s="65"/>
     </row>
     <row r="14" spans="1:10" ht="15">
       <c r="A14" s="8" t="str">
@@ -17180,18 +17150,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H14" s="65" t="str">
+      <c r="H14" s="65"/>
+      <c r="I14" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I14" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J14" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J14" s="65"/>
     </row>
     <row r="15" spans="1:10" ht="15">
       <c r="A15" s="8" t="str">
@@ -17207,18 +17171,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H15" s="65" t="str">
+      <c r="H15" s="65"/>
+      <c r="I15" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I15" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J15" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J15" s="65"/>
     </row>
     <row r="16" spans="1:10" ht="15">
       <c r="A16" s="8" t="str">
@@ -17234,18 +17192,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H16" s="65" t="str">
+      <c r="H16" s="65"/>
+      <c r="I16" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I16" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J16" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J16" s="65"/>
     </row>
     <row r="17" spans="1:10" ht="15">
       <c r="A17" s="8" t="str">
@@ -17261,18 +17213,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H17" s="65" t="str">
+      <c r="H17" s="65"/>
+      <c r="I17" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I17" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J17" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J17" s="65"/>
     </row>
     <row r="18" spans="1:10" ht="15" hidden="1">
       <c r="A18" s="8" t="str">
@@ -17288,18 +17234,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H18" s="65" t="str">
+      <c r="H18" s="65"/>
+      <c r="I18" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I18" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J18" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J18" s="65"/>
     </row>
     <row r="19" spans="1:10" ht="15" hidden="1">
       <c r="A19" s="8" t="str">
@@ -17315,18 +17255,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H19" s="65" t="str">
+      <c r="H19" s="65"/>
+      <c r="I19" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I19" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J19" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J19" s="65"/>
     </row>
     <row r="20" spans="1:10" ht="15" hidden="1">
       <c r="A20" s="8" t="str">
@@ -17342,18 +17276,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H20" s="65" t="str">
+      <c r="H20" s="65"/>
+      <c r="I20" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I20" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J20" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J20" s="65"/>
     </row>
     <row r="21" spans="1:10" ht="15" hidden="1">
       <c r="A21" s="8" t="str">
@@ -17369,18 +17297,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H21" s="65" t="str">
+      <c r="H21" s="65"/>
+      <c r="I21" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I21" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J21" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J21" s="65"/>
     </row>
     <row r="22" spans="1:10" ht="15">
       <c r="A22" s="8" t="str">
@@ -17396,18 +17318,12 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H22" s="65" t="str">
+      <c r="H22" s="65"/>
+      <c r="I22" s="17" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I22" s="17" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J22" s="65" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="J22" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="8" t="s">
@@ -17417,37 +17333,31 @@
         <v>1122</v>
       </c>
       <c r="C23" s="17">
-        <f t="shared" ref="C23:J23" si="4">IF(C6="","",SUM(C9:C22))</f>
+        <f t="shared" ref="C23:J23" si="2">IF(C6="","",SUM(C9:C22))</f>
         <v>0</v>
       </c>
       <c r="D23" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E23" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F23" s="17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G23" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="17"/>
       <c r="I23" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J23" s="17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" ht="15">
       <c r="A24" s="7"/>
@@ -17468,10 +17378,7 @@
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="65" t="str">
-        <f>IF(OR(G$6="", B25=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="G25" s="65"/>
       <c r="H25" s="65" t="str">
         <f>IF(OR(H$6="", $B25=""),"",SUM(E25:F25)-C25)</f>
         <v/>
@@ -17480,10 +17387,7 @@
         <f>IF(OR(I$6="", B25=""),"",SUM(G25:H25))</f>
         <v/>
       </c>
-      <c r="J25" s="65" t="str">
-        <f t="shared" ref="J25:J36" si="5">IF(OR(J$6="", $B25=""),"",0)</f>
-        <v/>
-      </c>
+      <c r="J25" s="65"/>
     </row>
     <row r="26" spans="1:10" ht="15">
       <c r="A26" s="8" t="str">
@@ -17495,22 +17399,16 @@
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
-      <c r="G26" s="65" t="str">
-        <f t="shared" ref="G26:G36" si="6">IF(OR(G$6="", B26=""),"",0)</f>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65" t="str">
+        <f t="shared" ref="H26:H36" si="3">IF(OR(H$6="", $B26=""),"",SUM(E26:F26)-C26)</f>
         <v/>
       </c>
-      <c r="H26" s="65" t="str">
-        <f t="shared" ref="H26:H36" si="7">IF(OR(H$6="", $B26=""),"",SUM(E26:F26)-C26)</f>
+      <c r="I26" s="17" t="str">
+        <f t="shared" ref="I26:I36" si="4">IF(OR(I$6="", B26=""),"",SUM(G26:H26))</f>
         <v/>
       </c>
-      <c r="I26" s="17" t="str">
-        <f t="shared" ref="I26:I36" si="8">IF(OR(I$6="", B26=""),"",SUM(G26:H26))</f>
-        <v/>
-      </c>
-      <c r="J26" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J26" s="65"/>
     </row>
     <row r="27" spans="1:10" ht="15">
       <c r="A27" s="8" t="str">
@@ -17522,22 +17420,16 @@
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H27" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I27" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I27" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J27" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J27" s="65"/>
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="8" t="str">
@@ -17549,22 +17441,16 @@
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H28" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I28" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I28" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J28" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J28" s="65"/>
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="8" t="str">
@@ -17576,22 +17462,16 @@
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H29" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I29" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I29" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J29" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J29" s="65"/>
     </row>
     <row r="30" spans="1:10" ht="15">
       <c r="A30" s="8" t="str">
@@ -17603,22 +17483,16 @@
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
-      <c r="G30" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H30" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I30" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I30" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J30" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J30" s="65"/>
     </row>
     <row r="31" spans="1:10" ht="15">
       <c r="A31" s="8" t="str">
@@ -17630,22 +17504,16 @@
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
-      <c r="G31" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H31" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I31" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I31" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J31" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J31" s="65"/>
     </row>
     <row r="32" spans="1:10" ht="15" hidden="1">
       <c r="A32" s="8" t="str">
@@ -17657,22 +17525,16 @@
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
-      <c r="G32" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H32" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I32" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I32" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J32" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J32" s="65"/>
     </row>
     <row r="33" spans="1:10" ht="15" hidden="1">
       <c r="A33" s="8" t="str">
@@ -17684,22 +17546,16 @@
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
-      <c r="G33" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H33" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I33" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I33" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J33" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J33" s="65"/>
     </row>
     <row r="34" spans="1:10" ht="15" hidden="1">
       <c r="A34" s="8" t="str">
@@ -17711,22 +17567,16 @@
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
-      <c r="G34" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H34" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I34" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I34" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J34" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J34" s="65"/>
     </row>
     <row r="35" spans="1:10" ht="15" hidden="1">
       <c r="A35" s="8" t="str">
@@ -17738,22 +17588,16 @@
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H35" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I35" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I35" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J35" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J35" s="65"/>
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="8" t="str">
@@ -17765,22 +17609,16 @@
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
-      <c r="G36" s="65" t="str">
-        <f t="shared" si="6"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="H36" s="65" t="str">
-        <f t="shared" si="7"/>
+      <c r="I36" s="17" t="str">
+        <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I36" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="J36" s="65" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="J36" s="65"/>
     </row>
     <row r="37" spans="1:10" s="52" customFormat="1" ht="15">
       <c r="A37" s="8" t="s">
@@ -17798,29 +17636,23 @@
         <v>0</v>
       </c>
       <c r="E37" s="17">
-        <f t="shared" ref="E37" si="9">IF(E6="","",SUM(E25:E36))</f>
+        <f t="shared" ref="E37" si="5">IF(E6="","",SUM(E25:E36))</f>
         <v>0</v>
       </c>
       <c r="F37" s="17">
-        <f t="shared" ref="F37:G37" si="10">IF(F6="","",SUM(F25:F36))</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="17">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
+        <f t="shared" ref="F37:G37" si="6">IF(F6="","",SUM(F25:F36))</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="17"/>
       <c r="H37" s="17">
-        <f t="shared" ref="H37" si="11">IF(H6="","",SUM(H25:H36))</f>
+        <f t="shared" ref="H37" si="7">IF(H6="","",SUM(H25:H36))</f>
         <v>0</v>
       </c>
       <c r="I37" s="17">
         <f>IF(I$6="","",SUM(I25:I36))</f>
         <v>0</v>
       </c>
-      <c r="J37" s="17">
-        <f t="shared" ref="J37" si="12">IF(J6="","",SUM(J25:J36))</f>
-        <v>0</v>
-      </c>
+      <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10" ht="15">
       <c r="A38" s="8" t="s">
@@ -17834,33 +17666,30 @@
         <v>0</v>
       </c>
       <c r="D38" s="23">
-        <f t="shared" ref="D38:G38" si="13">D23+D37</f>
+        <f t="shared" ref="D38:G38" si="8">D23+D37</f>
         <v>0</v>
       </c>
       <c r="E38" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F38" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G38" s="23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H38" s="25">
-        <f t="shared" ref="H38:I38" si="14">IF(H$6="","",H23+H37)</f>
+        <f t="shared" ref="H38:I38" si="9">IF(H$6="","",H23+H37)</f>
         <v>0</v>
       </c>
       <c r="I38" s="25">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="25">
-        <f>IF(J$6="","",J23+J37)</f>
-        <v>0</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="25"/>
     </row>
     <row r="39" spans="1:10" ht="15">
       <c r="A39" s="7"/>
@@ -17918,19 +17747,19 @@
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
       <c r="G42" s="65" t="str">
-        <f t="shared" ref="G42:H49" si="15">IF(OR(G$6="", B42=""),"",0)</f>
+        <f t="shared" ref="G42:H49" si="10">IF(OR(G$6="", B42=""),"",0)</f>
         <v/>
       </c>
       <c r="H42" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I42" s="17" t="str">
-        <f t="shared" ref="I42:I49" si="16">IF(OR($E$6="", F42=""),"",SUM(G42:H42))</f>
+        <f t="shared" ref="I42:I49" si="11">IF(OR($E$6="", F42=""),"",SUM(G42:H42))</f>
         <v/>
       </c>
       <c r="J42" s="65" t="str">
-        <f t="shared" ref="J42:J49" si="17">IF(OR(J$6="", E42=""),"",SUM(D42:F42)-C42)</f>
+        <f t="shared" ref="J42:J49" si="12">IF(OR(J$6="", E42=""),"",SUM(D42:F42)-C42)</f>
         <v/>
       </c>
     </row>
@@ -17945,19 +17774,19 @@
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H43" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I43" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J43" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -17972,19 +17801,19 @@
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H44" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I44" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J44" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -17999,19 +17828,19 @@
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
       <c r="G45" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H45" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I45" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J45" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -18026,19 +17855,19 @@
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
       <c r="G46" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H46" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I46" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J46" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -18053,19 +17882,19 @@
       <c r="E47" s="20"/>
       <c r="F47" s="20"/>
       <c r="G47" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H47" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I47" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J47" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -18080,19 +17909,19 @@
       <c r="E48" s="20"/>
       <c r="F48" s="20"/>
       <c r="G48" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H48" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I48" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J48" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -18107,19 +17936,19 @@
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
       <c r="G49" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H49" s="65" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I49" s="17" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J49" s="65" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -18139,27 +17968,27 @@
         <v>0</v>
       </c>
       <c r="E50" s="25">
-        <f t="shared" ref="E50" si="18">IF(E6="","",SUM(E41:E49))</f>
+        <f t="shared" ref="E50" si="13">IF(E6="","",SUM(E41:E49))</f>
         <v>0</v>
       </c>
       <c r="F50" s="25">
-        <f t="shared" ref="F50:G50" si="19">IF(F6="","",SUM(F41:F49))</f>
+        <f t="shared" ref="F50:G50" si="14">IF(F6="","",SUM(F41:F49))</f>
         <v>0</v>
       </c>
       <c r="G50" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H50" s="25">
-        <f t="shared" ref="H50:I50" si="20">IF(H6="","",SUM(H41:H49))</f>
+        <f t="shared" ref="H50:I50" si="15">IF(H6="","",SUM(H41:H49))</f>
         <v>0</v>
       </c>
       <c r="I50" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="J50" s="25">
-        <f t="shared" ref="J50" si="21">IF(J6="","",SUM(J41:J49))</f>
+        <f t="shared" ref="J50" si="16">IF(J6="","",SUM(J41:J49))</f>
         <v>0</v>
       </c>
     </row>
@@ -18206,7 +18035,7 @@
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
       <c r="I54" s="17" t="str">
-        <f t="shared" ref="I54:I63" si="22">IF(OR($E$6="", F54=""),"",SUM(G54:H54))</f>
+        <f t="shared" ref="I54:I63" si="17">IF(OR($E$6="", F54=""),"",SUM(G54:H54))</f>
         <v/>
       </c>
       <c r="J54" s="20"/>
@@ -18224,7 +18053,7 @@
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
       <c r="I55" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J55" s="20"/>
@@ -18242,7 +18071,7 @@
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
       <c r="I56" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J56" s="20"/>
@@ -18260,7 +18089,7 @@
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
       <c r="I57" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J57" s="20"/>
@@ -18278,7 +18107,7 @@
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J58" s="20"/>
@@ -18296,7 +18125,7 @@
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
       <c r="I59" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J59" s="20"/>
@@ -18314,7 +18143,7 @@
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
       <c r="I60" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J60" s="20"/>
@@ -18332,7 +18161,7 @@
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
       <c r="I61" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J61" s="20"/>
@@ -18368,7 +18197,7 @@
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
       <c r="I63" s="17" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J63" s="20"/>
@@ -18425,7 +18254,7 @@
       <c r="G66" s="20"/>
       <c r="H66" s="20"/>
       <c r="I66" s="17" t="str">
-        <f t="shared" ref="I66:I70" si="23">IF(OR($E$6="", F66=""),"",SUM(G66:H66))</f>
+        <f t="shared" ref="I66:I70" si="18">IF(OR($E$6="", F66=""),"",SUM(G66:H66))</f>
         <v/>
       </c>
       <c r="J66" s="20"/>
@@ -18443,7 +18272,7 @@
       <c r="G67" s="20"/>
       <c r="H67" s="20"/>
       <c r="I67" s="17" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J67" s="20"/>
@@ -18461,7 +18290,7 @@
       <c r="G68" s="20"/>
       <c r="H68" s="20"/>
       <c r="I68" s="17" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J68" s="20"/>
@@ -18479,7 +18308,7 @@
       <c r="G69" s="20"/>
       <c r="H69" s="20"/>
       <c r="I69" s="17" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J69" s="20"/>
@@ -18497,7 +18326,7 @@
       <c r="G70" s="20"/>
       <c r="H70" s="20"/>
       <c r="I70" s="17" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J70" s="20"/>
@@ -18592,7 +18421,7 @@
       <c r="G75" s="20"/>
       <c r="H75" s="20"/>
       <c r="I75" s="17" t="str">
-        <f t="shared" ref="I75:I77" si="24">IF(OR($E$6="", F75=""),"",SUM(G75:H75))</f>
+        <f t="shared" ref="I75:I77" si="19">IF(OR($E$6="", F75=""),"",SUM(G75:H75))</f>
         <v/>
       </c>
       <c r="J75" s="20"/>
@@ -18611,7 +18440,7 @@
       <c r="G76" s="20"/>
       <c r="H76" s="20"/>
       <c r="I76" s="17" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="J76" s="20"/>
@@ -18630,7 +18459,7 @@
       <c r="G77" s="20"/>
       <c r="H77" s="20"/>
       <c r="I77" s="17" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="J77" s="20"/>
@@ -18773,7 +18602,7 @@
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B22 B25:B36 B41:B49" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
       <formula1>program_revenues</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
functionality for statement of activities
</commit_message>
<xml_diff>
--- a/static/input_files/acfrs/example_template.xlsx
+++ b/static/input_files/acfrs/example_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrinawheelan/Desktop/Code/CLOSUP/process_xbrl/process-xbrl/static/input_files/acfrs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D807F27-77E8-D543-A613-6F1476C70B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908DFE4B-89B3-384D-853E-FBC5105F040A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2540" yWindow="500" windowWidth="24180" windowHeight="17500" tabRatio="834" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5126,9 +5126,6 @@
     <t>City of Clayton, California</t>
   </si>
   <si>
-    <t>ProgramRevenues,Expenses,NetExpenseRevenue</t>
-  </si>
-  <si>
     <t>National Forest Reserve Taxes</t>
   </si>
   <si>
@@ -5310,6 +5307,9 @@
   </si>
   <si>
     <t>Grants and Entitlements Not Restricted for Specific Programs</t>
+  </si>
+  <si>
+    <t>acfr:ProgramRevenues,acfr:Expenses,acfr:NetExpenseRevenue</t>
   </si>
 </sst>
 </file>
@@ -5775,7 +5775,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5955,6 +5955,14 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5964,16 +5972,6 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -5981,6 +5979,30 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
   <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -6112,30 +6134,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -14155,7 +14153,7 @@
         <v>1548</v>
       </c>
       <c r="B112" s="79" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="C112" s="79" t="s">
         <v>1549</v>
@@ -14166,7 +14164,7 @@
         <v>1548</v>
       </c>
       <c r="B113" s="79" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="C113" s="79" t="s">
         <v>1550</v>
@@ -14177,7 +14175,7 @@
         <v>1548</v>
       </c>
       <c r="B114" s="79" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="C114" s="79" t="s">
         <v>1551</v>
@@ -14188,7 +14186,7 @@
         <v>1548</v>
       </c>
       <c r="B115" s="79" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="C115" s="79" t="s">
         <v>1552</v>
@@ -14199,7 +14197,7 @@
         <v>1548</v>
       </c>
       <c r="B116" s="79" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="C116" s="79" t="s">
         <v>1553</v>
@@ -14210,7 +14208,7 @@
         <v>1548</v>
       </c>
       <c r="B117" s="79" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="C117" s="79" t="s">
         <v>1554</v>
@@ -14221,7 +14219,7 @@
         <v>1548</v>
       </c>
       <c r="B118" s="79" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="C118" s="79" t="s">
         <v>1555</v>
@@ -14232,7 +14230,7 @@
         <v>1548</v>
       </c>
       <c r="B119" s="79" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="C119" s="79" t="s">
         <v>1556</v>
@@ -14243,7 +14241,7 @@
         <v>1548</v>
       </c>
       <c r="B120" s="79" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="C120" s="79" t="s">
         <v>1557</v>
@@ -14254,7 +14252,7 @@
         <v>1548</v>
       </c>
       <c r="B121" s="79" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="C121" s="79" t="s">
         <v>1558</v>
@@ -14265,7 +14263,7 @@
         <v>1548</v>
       </c>
       <c r="B122" s="79" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="C122" s="79" t="s">
         <v>1559</v>
@@ -14276,7 +14274,7 @@
         <v>1548</v>
       </c>
       <c r="B123" s="79" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="C123" s="79" t="s">
         <v>1560</v>
@@ -14287,7 +14285,7 @@
         <v>1548</v>
       </c>
       <c r="B124" s="79" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="C124" s="79" t="s">
         <v>1561</v>
@@ -14298,7 +14296,7 @@
         <v>1548</v>
       </c>
       <c r="B125" s="79" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="C125" s="79" t="s">
         <v>1562</v>
@@ -14309,7 +14307,7 @@
         <v>1548</v>
       </c>
       <c r="B126" s="79" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="C126" s="79" t="s">
         <v>1563</v>
@@ -14320,7 +14318,7 @@
         <v>1548</v>
       </c>
       <c r="B127" s="79" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="C127" s="79" t="s">
         <v>1564</v>
@@ -14331,7 +14329,7 @@
         <v>1548</v>
       </c>
       <c r="B128" s="79" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="C128" s="79" t="s">
         <v>1565</v>
@@ -14342,7 +14340,7 @@
         <v>1548</v>
       </c>
       <c r="B129" s="79" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="C129" s="79" t="s">
         <v>1566</v>
@@ -14353,7 +14351,7 @@
         <v>1548</v>
       </c>
       <c r="B130" s="79" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="C130" s="79" t="s">
         <v>1567</v>
@@ -14364,7 +14362,7 @@
         <v>1548</v>
       </c>
       <c r="B131" s="79" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="C131" s="79" t="s">
         <v>1568</v>
@@ -14375,7 +14373,7 @@
         <v>1548</v>
       </c>
       <c r="B132" s="79" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="C132" s="79" t="s">
         <v>1569</v>
@@ -14386,7 +14384,7 @@
         <v>1548</v>
       </c>
       <c r="B133" s="79" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="C133" s="79" t="s">
         <v>1570</v>
@@ -14397,7 +14395,7 @@
         <v>1548</v>
       </c>
       <c r="B134" s="79" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="C134" s="79" t="s">
         <v>1571</v>
@@ -14408,7 +14406,7 @@
         <v>1548</v>
       </c>
       <c r="B135" s="79" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="C135" s="79" t="s">
         <v>1572</v>
@@ -14419,7 +14417,7 @@
         <v>1548</v>
       </c>
       <c r="B136" s="79" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="C136" s="79" t="s">
         <v>1573</v>
@@ -14430,7 +14428,7 @@
         <v>1548</v>
       </c>
       <c r="B137" s="79" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="C137" s="79" t="s">
         <v>1574</v>
@@ -14441,7 +14439,7 @@
         <v>1548</v>
       </c>
       <c r="B138" s="79" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="C138" s="79" t="s">
         <v>1575</v>
@@ -14452,7 +14450,7 @@
         <v>1548</v>
       </c>
       <c r="B139" s="79" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="C139" s="79" t="s">
         <v>1576</v>
@@ -14463,7 +14461,7 @@
         <v>1548</v>
       </c>
       <c r="B140" s="79" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="C140" s="79" t="s">
         <v>1577</v>
@@ -14474,7 +14472,7 @@
         <v>1548</v>
       </c>
       <c r="B141" s="79" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="C141" s="79" t="s">
         <v>1578</v>
@@ -14485,7 +14483,7 @@
         <v>1548</v>
       </c>
       <c r="B142" s="79" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="C142" s="79" t="s">
         <v>1579</v>
@@ -14496,7 +14494,7 @@
         <v>1548</v>
       </c>
       <c r="B143" s="79" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="C143" s="79" t="s">
         <v>1552</v>
@@ -14507,7 +14505,7 @@
         <v>1548</v>
       </c>
       <c r="B144" s="79" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="C144" s="79" t="s">
         <v>1580</v>
@@ -14518,7 +14516,7 @@
         <v>1548</v>
       </c>
       <c r="B145" s="79" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="C145" s="79" t="s">
         <v>1581</v>
@@ -14529,7 +14527,7 @@
         <v>1548</v>
       </c>
       <c r="B146" s="79" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="C146" s="79" t="s">
         <v>1582</v>
@@ -14540,7 +14538,7 @@
         <v>1548</v>
       </c>
       <c r="B147" s="79" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="C147" s="79" t="s">
         <v>1583</v>
@@ -14573,7 +14571,7 @@
         <v>1548</v>
       </c>
       <c r="B150" s="79" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="C150" s="79" t="s">
         <v>1588</v>
@@ -14584,7 +14582,7 @@
         <v>1548</v>
       </c>
       <c r="B151" s="79" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="C151" s="79" t="s">
         <v>1589</v>
@@ -14595,7 +14593,7 @@
         <v>1548</v>
       </c>
       <c r="B152" s="79" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="C152" s="79" t="s">
         <v>1590</v>
@@ -14617,7 +14615,7 @@
         <v>1548</v>
       </c>
       <c r="B154" s="79" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="C154" s="79" t="s">
         <v>1593</v>
@@ -14628,7 +14626,7 @@
         <v>1548</v>
       </c>
       <c r="B155" s="79" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="C155" s="79" t="s">
         <v>1594</v>
@@ -14639,7 +14637,7 @@
         <v>1548</v>
       </c>
       <c r="B156" s="79" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="C156" s="79" t="s">
         <v>1595</v>
@@ -14650,7 +14648,7 @@
         <v>1548</v>
       </c>
       <c r="B157" s="79" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="C157" s="79" t="s">
         <v>1596</v>
@@ -14672,7 +14670,7 @@
         <v>1548</v>
       </c>
       <c r="B159" s="79" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="C159" s="79" t="s">
         <v>1599</v>
@@ -14694,7 +14692,7 @@
         <v>1548</v>
       </c>
       <c r="B161" s="79" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="C161" s="79" t="s">
         <v>1602</v>
@@ -14705,7 +14703,7 @@
         <v>1548</v>
       </c>
       <c r="B162" s="79" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="C162" s="79" t="s">
         <v>1603</v>
@@ -14804,7 +14802,7 @@
         <v>1548</v>
       </c>
       <c r="B171" s="79" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="C171" s="79" t="s">
         <v>1219</v>
@@ -14815,7 +14813,7 @@
         <v>1548</v>
       </c>
       <c r="B172" s="79" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="C172" s="79" t="s">
         <v>1604</v>
@@ -14826,7 +14824,7 @@
         <v>1548</v>
       </c>
       <c r="B173" s="79" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C173" s="79" t="s">
         <v>1605</v>
@@ -14837,7 +14835,7 @@
         <v>1548</v>
       </c>
       <c r="B174" s="79" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C174" s="79" t="s">
         <v>1606</v>
@@ -14859,7 +14857,7 @@
         <v>1548</v>
       </c>
       <c r="B176" s="79" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C176" s="79" t="s">
         <v>1606</v>
@@ -14881,7 +14879,7 @@
         <v>1548</v>
       </c>
       <c r="B178" s="79" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="C178" s="79" t="s">
         <v>1611</v>
@@ -14914,7 +14912,7 @@
         <v>1548</v>
       </c>
       <c r="B181" s="79" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="C181" s="79" t="s">
         <v>1616</v>
@@ -14925,7 +14923,7 @@
         <v>1548</v>
       </c>
       <c r="B182" s="79" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="C182" s="79" t="s">
         <v>1617</v>
@@ -14936,7 +14934,7 @@
         <v>1548</v>
       </c>
       <c r="B183" s="79" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="C183" s="79" t="s">
         <v>1618</v>
@@ -14947,7 +14945,7 @@
         <v>1548</v>
       </c>
       <c r="B184" s="79" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="C184" s="79" t="s">
         <v>1619</v>
@@ -14958,7 +14956,7 @@
         <v>1548</v>
       </c>
       <c r="B185" s="79" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="C185" s="79" t="s">
         <v>1620</v>
@@ -14969,7 +14967,7 @@
         <v>1548</v>
       </c>
       <c r="B186" s="79" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="C186" s="79" t="s">
         <v>1621</v>
@@ -14980,7 +14978,7 @@
         <v>1548</v>
       </c>
       <c r="B187" s="79" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="C187" s="79" t="s">
         <v>1622</v>
@@ -14991,7 +14989,7 @@
         <v>1548</v>
       </c>
       <c r="B188" s="79" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="C188" s="79" t="s">
         <v>1623</v>
@@ -15002,7 +15000,7 @@
         <v>1548</v>
       </c>
       <c r="B189" s="79" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="C189" s="79" t="s">
         <v>1624</v>
@@ -15013,7 +15011,7 @@
         <v>1548</v>
       </c>
       <c r="B190" s="79" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="C190" s="79" t="s">
         <v>1625</v>
@@ -15024,7 +15022,7 @@
         <v>1548</v>
       </c>
       <c r="B191" s="79" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="C191" s="79" t="s">
         <v>1626</v>
@@ -16857,7 +16855,7 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23 C37 C50 C65 C76:C77 C89 C101 D6:F101">
+  <conditionalFormatting sqref="D6:F101 C23 C37 C50 C65 C76:C77 C89 C101">
     <cfRule type="expression" dxfId="29" priority="2" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
@@ -16901,7 +16899,7 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
@@ -17047,7 +17045,7 @@
       </c>
       <c r="H9" s="65"/>
       <c r="I9" s="17" t="str">
-        <f>IF(OR($E$6="", B9=""),"",SUM(G9:H9))</f>
+        <f>IF(OR(I$6="", B9=""),"",SUM(G9:H9))</f>
         <v/>
       </c>
       <c r="J9" s="65"/>
@@ -17068,7 +17066,7 @@
       </c>
       <c r="H10" s="65"/>
       <c r="I10" s="17" t="str">
-        <f>IF(OR($E$6="", B10=""),"",SUM(G10:H10))</f>
+        <f t="shared" ref="I10:I22" si="0">IF(OR(I$6="", B10=""),"",SUM(G10:H10))</f>
         <v/>
       </c>
       <c r="J10" s="65"/>
@@ -17084,12 +17082,12 @@
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="65" t="str">
-        <f t="shared" ref="G11:G22" si="0">IF(OR(G$6="", B11=""),"",SUM(E11:F11) - C11)</f>
+        <f t="shared" ref="G11:G22" si="1">IF(OR(G$6="", B11=""),"",SUM(E11:F11) - C11)</f>
         <v/>
       </c>
       <c r="H11" s="65"/>
       <c r="I11" s="17" t="str">
-        <f t="shared" ref="I10:I22" si="1">IF(OR($E$6="", B11=""),"",SUM(G11:H11))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J11" s="65"/>
@@ -17105,12 +17103,12 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H12" s="65"/>
       <c r="I12" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J12" s="65"/>
@@ -17126,12 +17124,12 @@
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H13" s="65"/>
       <c r="I13" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J13" s="65"/>
@@ -17147,12 +17145,12 @@
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H14" s="65"/>
       <c r="I14" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J14" s="65"/>
@@ -17168,12 +17166,12 @@
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H15" s="65"/>
       <c r="I15" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J15" s="65"/>
@@ -17189,12 +17187,12 @@
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
       <c r="G16" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H16" s="65"/>
       <c r="I16" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J16" s="65"/>
@@ -17210,12 +17208,12 @@
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
       <c r="G17" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H17" s="65"/>
       <c r="I17" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J17" s="65"/>
@@ -17231,12 +17229,12 @@
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
       <c r="G18" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H18" s="65"/>
       <c r="I18" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J18" s="65"/>
@@ -17252,12 +17250,12 @@
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H19" s="65"/>
       <c r="I19" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J19" s="65"/>
@@ -17273,12 +17271,12 @@
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H20" s="65"/>
       <c r="I20" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J20" s="65"/>
@@ -17294,12 +17292,12 @@
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="65" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H21" s="65"/>
       <c r="I21" s="17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="J21" s="65"/>
@@ -17315,25 +17313,25 @@
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="65" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="H22" s="65"/>
+      <c r="I22" s="17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H22" s="65"/>
-      <c r="I22" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="J22" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="15">
       <c r="A23" s="8" t="s">
-        <v>1682</v>
+        <v>1743</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>1122</v>
       </c>
       <c r="C23" s="17">
-        <f t="shared" ref="C23:J23" si="2">IF(C6="","",SUM(C9:C22))</f>
+        <f t="shared" ref="C23:I23" si="2">IF(C6="","",SUM(C9:C22))</f>
         <v>0</v>
       </c>
       <c r="D23" s="17">
@@ -17384,7 +17382,7 @@
         <v/>
       </c>
       <c r="I25" s="17" t="str">
-        <f>IF(OR(I$6="", B25=""),"",SUM(G25:H25))</f>
+        <f t="shared" ref="I25:I36" si="3">IF(OR(I$6="", B25=""),"",SUM(G25:H25))</f>
         <v/>
       </c>
       <c r="J25" s="65"/>
@@ -17401,11 +17399,11 @@
       <c r="F26" s="20"/>
       <c r="G26" s="65"/>
       <c r="H26" s="65" t="str">
-        <f t="shared" ref="H26:H36" si="3">IF(OR(H$6="", $B26=""),"",SUM(E26:F26)-C26)</f>
+        <f t="shared" ref="H26:H36" si="4">IF(OR(H$6="", $B26=""),"",SUM(E26:F26)-C26)</f>
         <v/>
       </c>
       <c r="I26" s="17" t="str">
-        <f t="shared" ref="I26:I36" si="4">IF(OR(I$6="", B26=""),"",SUM(G26:H26))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="J26" s="65"/>
@@ -17422,11 +17420,11 @@
       <c r="F27" s="20"/>
       <c r="G27" s="65"/>
       <c r="H27" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I27" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I27" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J27" s="65"/>
@@ -17443,11 +17441,11 @@
       <c r="F28" s="20"/>
       <c r="G28" s="65"/>
       <c r="H28" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I28" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I28" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J28" s="65"/>
@@ -17464,11 +17462,11 @@
       <c r="F29" s="20"/>
       <c r="G29" s="65"/>
       <c r="H29" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I29" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I29" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J29" s="65"/>
@@ -17485,11 +17483,11 @@
       <c r="F30" s="19"/>
       <c r="G30" s="65"/>
       <c r="H30" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I30" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I30" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J30" s="65"/>
@@ -17506,11 +17504,11 @@
       <c r="F31" s="19"/>
       <c r="G31" s="65"/>
       <c r="H31" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I31" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I31" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J31" s="65"/>
@@ -17527,11 +17525,11 @@
       <c r="F32" s="19"/>
       <c r="G32" s="65"/>
       <c r="H32" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I32" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I32" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J32" s="65"/>
@@ -17548,11 +17546,11 @@
       <c r="F33" s="19"/>
       <c r="G33" s="65"/>
       <c r="H33" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I33" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I33" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J33" s="65"/>
@@ -17569,11 +17567,11 @@
       <c r="F34" s="19"/>
       <c r="G34" s="65"/>
       <c r="H34" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I34" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I34" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J34" s="65"/>
@@ -17590,11 +17588,11 @@
       <c r="F35" s="19"/>
       <c r="G35" s="65"/>
       <c r="H35" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I35" s="17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I35" s="17" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="J35" s="65"/>
@@ -17611,18 +17609,18 @@
       <c r="F36" s="19"/>
       <c r="G36" s="65"/>
       <c r="H36" s="65" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="I36" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="I36" s="17" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="J36" s="65"/>
     </row>
     <row r="37" spans="1:10" s="52" customFormat="1" ht="15">
       <c r="A37" s="8" t="s">
-        <v>1682</v>
+        <v>1743</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>1129</v>
@@ -17640,7 +17638,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="17">
-        <f t="shared" ref="F37:G37" si="6">IF(F6="","",SUM(F25:F36))</f>
+        <f t="shared" ref="F37" si="6">IF(F6="","",SUM(F25:F36))</f>
         <v>0</v>
       </c>
       <c r="G37" s="17"/>
@@ -17656,7 +17654,7 @@
     </row>
     <row r="38" spans="1:10" ht="15">
       <c r="A38" s="8" t="s">
-        <v>1682</v>
+        <v>1743</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>1123</v>
@@ -17730,7 +17728,10 @@
         <f>IF(OR(H$6="", C41=""),"",0)</f>
         <v/>
       </c>
-      <c r="I41" s="17"/>
+      <c r="I41" s="17" t="str">
+        <f t="shared" ref="I41:I49" si="10">IF(OR(I$6="", B41=""),"",SUM(G41:H41))</f>
+        <v/>
+      </c>
       <c r="J41" s="65" t="str">
         <f>IF(OR(J$6="", E41=""),"",SUM(D41:F41)-C41)</f>
         <v/>
@@ -17747,15 +17748,15 @@
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
       <c r="G42" s="65" t="str">
-        <f t="shared" ref="G42:H49" si="10">IF(OR(G$6="", B42=""),"",0)</f>
+        <f t="shared" ref="G42:H49" si="11">IF(OR(G$6="", B42=""),"",0)</f>
         <v/>
       </c>
       <c r="H42" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I42" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I42" s="17" t="str">
-        <f t="shared" ref="I42:I49" si="11">IF(OR($E$6="", F42=""),"",SUM(G42:H42))</f>
         <v/>
       </c>
       <c r="J42" s="65" t="str">
@@ -17774,15 +17775,15 @@
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H43" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I43" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H43" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I43" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J43" s="65" t="str">
@@ -17801,15 +17802,15 @@
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H44" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I44" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H44" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I44" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J44" s="65" t="str">
@@ -17828,15 +17829,15 @@
       <c r="E45" s="20"/>
       <c r="F45" s="20"/>
       <c r="G45" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H45" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I45" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H45" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I45" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J45" s="65" t="str">
@@ -17855,15 +17856,15 @@
       <c r="E46" s="20"/>
       <c r="F46" s="20"/>
       <c r="G46" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H46" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I46" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H46" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I46" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J46" s="65" t="str">
@@ -17882,15 +17883,15 @@
       <c r="E47" s="20"/>
       <c r="F47" s="20"/>
       <c r="G47" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H47" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I47" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H47" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I47" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J47" s="65" t="str">
@@ -17909,15 +17910,15 @@
       <c r="E48" s="20"/>
       <c r="F48" s="20"/>
       <c r="G48" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H48" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I48" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H48" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I48" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J48" s="65" t="str">
@@ -17936,15 +17937,15 @@
       <c r="E49" s="20"/>
       <c r="F49" s="20"/>
       <c r="G49" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="H49" s="65" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="I49" s="17" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="H49" s="65" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="I49" s="17" t="str">
-        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J49" s="65" t="str">
@@ -17954,7 +17955,7 @@
     </row>
     <row r="50" spans="1:10" ht="15">
       <c r="A50" s="8" t="s">
-        <v>1682</v>
+        <v>1743</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>1128</v>
@@ -18028,14 +18029,14 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B54" s="18"/>
-      <c r="C54" s="101"/>
-      <c r="D54" s="102"/>
-      <c r="E54" s="102"/>
-      <c r="F54" s="102"/>
+      <c r="C54" s="98"/>
+      <c r="D54" s="99"/>
+      <c r="E54" s="99"/>
+      <c r="F54" s="99"/>
       <c r="G54" s="20"/>
       <c r="H54" s="20"/>
       <c r="I54" s="17" t="str">
-        <f t="shared" ref="I54:I63" si="17">IF(OR($E$6="", F54=""),"",SUM(G54:H54))</f>
+        <f t="shared" ref="I54:I63" si="17">IF(OR(I$6="", B54=""),"",SUM(G54:H54))</f>
         <v/>
       </c>
       <c r="J54" s="20"/>
@@ -18046,10 +18047,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B55" s="18"/>
-      <c r="C55" s="101"/>
-      <c r="D55" s="102"/>
-      <c r="E55" s="102"/>
-      <c r="F55" s="102"/>
+      <c r="C55" s="98"/>
+      <c r="D55" s="99"/>
+      <c r="E55" s="99"/>
+      <c r="F55" s="99"/>
       <c r="G55" s="20"/>
       <c r="H55" s="20"/>
       <c r="I55" s="17" t="str">
@@ -18064,10 +18065,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B56" s="18"/>
-      <c r="C56" s="101"/>
-      <c r="D56" s="102"/>
-      <c r="E56" s="102"/>
-      <c r="F56" s="102"/>
+      <c r="C56" s="98"/>
+      <c r="D56" s="99"/>
+      <c r="E56" s="99"/>
+      <c r="F56" s="99"/>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
       <c r="I56" s="17" t="str">
@@ -18082,10 +18083,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B57" s="18"/>
-      <c r="C57" s="101"/>
-      <c r="D57" s="102"/>
-      <c r="E57" s="102"/>
-      <c r="F57" s="102"/>
+      <c r="C57" s="98"/>
+      <c r="D57" s="99"/>
+      <c r="E57" s="99"/>
+      <c r="F57" s="99"/>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
       <c r="I57" s="17" t="str">
@@ -18100,10 +18101,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B58" s="18"/>
-      <c r="C58" s="101"/>
-      <c r="D58" s="102"/>
-      <c r="E58" s="102"/>
-      <c r="F58" s="102"/>
+      <c r="C58" s="98"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="99"/>
+      <c r="F58" s="99"/>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="17" t="str">
@@ -18118,10 +18119,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B59" s="18"/>
-      <c r="C59" s="101"/>
-      <c r="D59" s="102"/>
-      <c r="E59" s="102"/>
-      <c r="F59" s="102"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="99"/>
+      <c r="E59" s="99"/>
+      <c r="F59" s="99"/>
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
       <c r="I59" s="17" t="str">
@@ -18136,10 +18137,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B60" s="18"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="102"/>
-      <c r="E60" s="102"/>
-      <c r="F60" s="102"/>
+      <c r="C60" s="98"/>
+      <c r="D60" s="99"/>
+      <c r="E60" s="99"/>
+      <c r="F60" s="99"/>
       <c r="G60" s="20"/>
       <c r="H60" s="20"/>
       <c r="I60" s="17" t="str">
@@ -18154,10 +18155,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B61" s="18"/>
-      <c r="C61" s="101"/>
-      <c r="D61" s="102"/>
-      <c r="E61" s="102"/>
-      <c r="F61" s="102"/>
+      <c r="C61" s="98"/>
+      <c r="D61" s="99"/>
+      <c r="E61" s="99"/>
+      <c r="F61" s="99"/>
       <c r="G61" s="20"/>
       <c r="H61" s="20"/>
       <c r="I61" s="17" t="str">
@@ -18172,14 +18173,14 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B62" s="18"/>
-      <c r="C62" s="101"/>
-      <c r="D62" s="102"/>
-      <c r="E62" s="102"/>
-      <c r="F62" s="102"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="99"/>
+      <c r="E62" s="99"/>
+      <c r="F62" s="99"/>
       <c r="G62" s="20"/>
       <c r="H62" s="20"/>
       <c r="I62" s="17" t="str">
-        <f>IF(OR($E$6="", F62=""),"",SUM(G62:H62))</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J62" s="20"/>
@@ -18190,10 +18191,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B63" s="18"/>
-      <c r="C63" s="101"/>
-      <c r="D63" s="102"/>
-      <c r="E63" s="102"/>
-      <c r="F63" s="102"/>
+      <c r="C63" s="98"/>
+      <c r="D63" s="99"/>
+      <c r="E63" s="99"/>
+      <c r="F63" s="99"/>
       <c r="G63" s="20"/>
       <c r="H63" s="20"/>
       <c r="I63" s="17" t="str">
@@ -18235,10 +18236,8 @@
       <c r="B65" s="15" t="s">
         <v>1143</v>
       </c>
-      <c r="C65" s="103"/>
-      <c r="D65" s="103"/>
-      <c r="E65" s="104"/>
-      <c r="F65" s="104"/>
+      <c r="C65" s="100"/>
+      <c r="D65" s="100"/>
       <c r="I65" s="15"/>
     </row>
     <row r="66" spans="1:10" ht="15">
@@ -18247,14 +18246,14 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B66" s="18"/>
-      <c r="C66" s="101"/>
-      <c r="D66" s="102"/>
-      <c r="E66" s="102"/>
-      <c r="F66" s="102"/>
+      <c r="C66" s="98"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="99"/>
+      <c r="F66" s="99"/>
       <c r="G66" s="20"/>
       <c r="H66" s="20"/>
       <c r="I66" s="17" t="str">
-        <f t="shared" ref="I66:I70" si="18">IF(OR($E$6="", F66=""),"",SUM(G66:H66))</f>
+        <f t="shared" ref="I66:I70" si="18">IF(OR(I$6="", B66=""),"",SUM(G66:H66))</f>
         <v/>
       </c>
       <c r="J66" s="20"/>
@@ -18265,10 +18264,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B67" s="18"/>
-      <c r="C67" s="101"/>
-      <c r="D67" s="102"/>
-      <c r="E67" s="102"/>
-      <c r="F67" s="102"/>
+      <c r="C67" s="98"/>
+      <c r="D67" s="99"/>
+      <c r="E67" s="99"/>
+      <c r="F67" s="99"/>
       <c r="G67" s="20"/>
       <c r="H67" s="20"/>
       <c r="I67" s="17" t="str">
@@ -18283,10 +18282,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B68" s="18"/>
-      <c r="C68" s="101"/>
-      <c r="D68" s="102"/>
-      <c r="E68" s="102"/>
-      <c r="F68" s="102"/>
+      <c r="C68" s="98"/>
+      <c r="D68" s="99"/>
+      <c r="E68" s="99"/>
+      <c r="F68" s="99"/>
       <c r="G68" s="20"/>
       <c r="H68" s="20"/>
       <c r="I68" s="17" t="str">
@@ -18301,10 +18300,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B69" s="18"/>
-      <c r="C69" s="101"/>
-      <c r="D69" s="102"/>
-      <c r="E69" s="102"/>
-      <c r="F69" s="102"/>
+      <c r="C69" s="98"/>
+      <c r="D69" s="99"/>
+      <c r="E69" s="99"/>
+      <c r="F69" s="99"/>
       <c r="G69" s="20"/>
       <c r="H69" s="20"/>
       <c r="I69" s="17" t="str">
@@ -18319,10 +18318,10 @@
         <v>Choose from drop-down --&gt;</v>
       </c>
       <c r="B70" s="18"/>
-      <c r="C70" s="101"/>
-      <c r="D70" s="102"/>
-      <c r="E70" s="102"/>
-      <c r="F70" s="102"/>
+      <c r="C70" s="98"/>
+      <c r="D70" s="99"/>
+      <c r="E70" s="99"/>
+      <c r="F70" s="99"/>
       <c r="G70" s="20"/>
       <c r="H70" s="20"/>
       <c r="I70" s="17" t="str">
@@ -18387,21 +18386,15 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="C73" s="104"/>
-      <c r="D73" s="104"/>
-      <c r="E73" s="104"/>
-      <c r="F73" s="104"/>
-    </row>
     <row r="74" spans="1:10" ht="15">
       <c r="A74" s="7"/>
       <c r="B74" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C74" s="105"/>
-      <c r="D74" s="105"/>
-      <c r="E74" s="105"/>
-      <c r="F74" s="105"/>
+      <c r="C74" s="76"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="76"/>
+      <c r="F74" s="76"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
@@ -18414,15 +18407,15 @@
       <c r="B75" s="10" t="s">
         <v>1134</v>
       </c>
-      <c r="C75" s="101"/>
-      <c r="D75" s="102"/>
-      <c r="E75" s="102"/>
-      <c r="F75" s="102"/>
+      <c r="C75" s="98"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="99"/>
+      <c r="F75" s="99"/>
       <c r="G75" s="20"/>
       <c r="H75" s="20"/>
-      <c r="I75" s="17" t="str">
-        <f t="shared" ref="I75:I77" si="19">IF(OR($E$6="", F75=""),"",SUM(G75:H75))</f>
-        <v/>
+      <c r="I75" s="17">
+        <f>IF(I$6="","",SUM(G75:H75))</f>
+        <v>0</v>
       </c>
       <c r="J75" s="20"/>
     </row>
@@ -18433,15 +18426,15 @@
       <c r="B76" s="10" t="s">
         <v>1135</v>
       </c>
-      <c r="C76" s="101"/>
-      <c r="D76" s="102"/>
-      <c r="E76" s="102"/>
-      <c r="F76" s="102"/>
+      <c r="C76" s="98"/>
+      <c r="D76" s="99"/>
+      <c r="E76" s="99"/>
+      <c r="F76" s="99"/>
       <c r="G76" s="20"/>
       <c r="H76" s="20"/>
-      <c r="I76" s="17" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+      <c r="I76" s="17">
+        <f t="shared" ref="I76:I77" si="19">IF(I$6="","",SUM(G76:H76))</f>
+        <v>0</v>
       </c>
       <c r="J76" s="20"/>
     </row>
@@ -18452,15 +18445,15 @@
       <c r="B77" s="10" t="s">
         <v>1136</v>
       </c>
-      <c r="C77" s="101"/>
-      <c r="D77" s="102"/>
-      <c r="E77" s="102"/>
-      <c r="F77" s="102"/>
+      <c r="C77" s="98"/>
+      <c r="D77" s="99"/>
+      <c r="E77" s="99"/>
+      <c r="F77" s="99"/>
       <c r="G77" s="20"/>
       <c r="H77" s="20"/>
-      <c r="I77" s="17" t="str">
+      <c r="I77" s="17">
         <f t="shared" si="19"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="J77" s="20"/>
     </row>
@@ -18532,77 +18525,77 @@
     </row>
   </sheetData>
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
-  <conditionalFormatting sqref="C23 C37 C50 D74:H77 J74:J77 I74:I99 D53:G63">
-    <cfRule type="expression" dxfId="28" priority="46" stopIfTrue="1">
+  <conditionalFormatting sqref="C23 C37 C50 D53:G63 D74:H77 J74:J77 I74 I78:I99">
+    <cfRule type="expression" dxfId="28" priority="49" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:J64">
-    <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="34" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:J72">
-    <cfRule type="expression" dxfId="26" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
       <formula>C$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:F6 D39:G40 D52:F52 D50:G51 D41:F49">
-    <cfRule type="expression" dxfId="25" priority="43" stopIfTrue="1">
+  <conditionalFormatting sqref="D6:F6 D52:F52">
+    <cfRule type="expression" dxfId="25" priority="46" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65:J70">
-    <cfRule type="expression" dxfId="24" priority="13" stopIfTrue="1">
+  <conditionalFormatting sqref="D39:G51">
+    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39:H40 H50">
-    <cfRule type="expression" dxfId="23" priority="41" stopIfTrue="1">
+  <conditionalFormatting sqref="D65:J65 D66:H70 J66:J70">
+    <cfRule type="expression" dxfId="23" priority="16" stopIfTrue="1">
+      <formula>D$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39:H50">
+    <cfRule type="expression" dxfId="22" priority="5" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:J6 I39:I51 D7:I37">
-    <cfRule type="expression" dxfId="22" priority="36" stopIfTrue="1">
+  <conditionalFormatting sqref="H38:I38">
+    <cfRule type="expression" dxfId="21" priority="43" stopIfTrue="1">
+      <formula>H$6=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:J6 D7:I37 I39:I51">
+    <cfRule type="expression" dxfId="20" priority="39" stopIfTrue="1">
       <formula>D$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52:J63">
-    <cfRule type="expression" dxfId="21" priority="20" stopIfTrue="1">
+  <conditionalFormatting sqref="H52:J53 H54:H63 J54:J63">
+    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>H$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J8 H38:I38 J23:J24 J37:J40 J50">
-    <cfRule type="expression" dxfId="20" priority="40" stopIfTrue="1">
-      <formula>H$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J22">
-    <cfRule type="expression" dxfId="19" priority="6" stopIfTrue="1">
-      <formula>J$6=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J25:J36">
+  <conditionalFormatting sqref="J7:J50">
     <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
       <formula>J$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G41:G49">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
-      <formula>G$6=""</formula>
+  <conditionalFormatting sqref="I54:I63">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41:H49">
-    <cfRule type="expression" dxfId="16" priority="2" stopIfTrue="1">
-      <formula>H$6=""</formula>
+  <conditionalFormatting sqref="I66:I70">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J41:J49">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
-      <formula>J$6=""</formula>
+  <conditionalFormatting sqref="I75:I77">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>I$6=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B22 B25:B36 B41:B49" xr:uid="{F3C11D5E-2141-5546-AF1F-2279D6DA74D8}">
       <formula1>program_revenues</formula1>
     </dataValidation>
@@ -19981,7 +19974,7 @@
   <sheetProtection formatRows="0" insertRows="0" deleteRows="0"/>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="D7:I7 D8:J23 C23 D25:J36 C36 C37:J37 D38:J71 C60:J60 C70">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
       <formula>C$7=""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20309,12 +20302,12 @@
     </row>
     <row r="25" spans="1:5" ht="15">
       <c r="A25" s="7"/>
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99"/>
-      <c r="E25" s="100"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="103"/>
     </row>
     <row r="26" spans="1:5" ht="15">
       <c r="A26" s="8" t="str">
@@ -21331,31 +21324,31 @@
     <mergeCell ref="B25:E25"/>
   </mergeCells>
   <conditionalFormatting sqref="C102">
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="equal">
       <formula>$C$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>$C$102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102:E102">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102">
-    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="equal">
       <formula>$D$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="notEqual">
       <formula>$D$102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E102">
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>$E$102</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>$E$102</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22689,31 +22682,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
       <formula>$C$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>$C$101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101:E101">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D101">
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
       <formula>$D$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="notEqual">
       <formula>$D$101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E101">
-    <cfRule type="cellIs" dxfId="1" priority="6" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>$E$101</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>$E$101</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>